<commit_message>
Movement ecology paper updates
</commit_message>
<xml_diff>
--- a/Example_data/Output/Predictions/MovementEcologyPaper/Supporting_information_Table_S1.xlsx
+++ b/Example_data/Output/Predictions/MovementEcologyPaper/Supporting_information_Table_S1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnvanOsta\Documents\GitHub\ml4rt\Example_data\Output\Predictions\MovementEcologyPaper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s5236256\Documents\GitHub\ml4rt\Example_data\Output\Predictions\MovementEcologyPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12147F37-611A-4ADF-849A-9990F7E2C8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D0401-1E8E-40CE-8E40-9345B9B617E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{97B86A08-93E9-4AF4-A45D-724E995BAEA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{97B86A08-93E9-4AF4-A45D-724E995BAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="home_range_data" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="191">
   <si>
     <t>mean_UD_95_ha</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>2021 Dry Season</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
@@ -962,22 +968,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="23.86328125" customWidth="1"/>
-    <col min="10" max="10" width="14.46484375" customWidth="1"/>
-    <col min="12" max="12" width="7.86328125" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1065,7 @@
         <v>78.414709999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>177.888293</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>96.462708000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>44.128166999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>143.78634299999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>186.160428</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>55.730297</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>272.80046800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>88.507678999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>348.96044499999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>2.8084259999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>156.01434</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>110.584964</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>3.0431940000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>6.2083050000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1680,7 @@
         <v>28.186378000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>13.568818</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>42.632511999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>29.229849999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1838,7 +1844,7 @@
         <v>24.541298999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>6.6943669999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1920,7 +1926,7 @@
         <v>76.987814</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>17.125398000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>28.840544999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>55.799422999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>194.83432999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>331.69065899999998</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>125.29405800000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>108.143698</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>57.419719999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>540.90782799999999</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -2330,7 +2336,7 @@
         <v>12.892841000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>56.453218999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>32.344897000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>19.401958</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>33.864825000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>37.377065999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>161.45064199999999</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>182.164162</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>55.572181999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>167.65533199999999</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2740,7 +2746,7 @@
         <v>105.46352899999999</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>123.25519</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>2.0971380000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>123.43628200000001</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>262.25954300000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>155.230773</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>104.034774</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -3027,7 +3033,7 @@
         <v>408.376261</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>219.70862399999999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -3109,7 +3115,7 @@
         <v>203.03821500000001</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>16.425597</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>195.592465</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>10.759765</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>34.293087999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>204.55538200000001</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -3355,7 +3361,7 @@
         <v>77.051287000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>202.44556399999999</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -3437,7 +3443,7 @@
         <v>23.131274999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -3478,7 +3484,7 @@
         <v>314.93723</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>479.96772900000002</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>452.14053699999999</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -3601,7 +3607,7 @@
         <v>7.6868590000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -3642,7 +3648,7 @@
         <v>17.447813</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -3683,7 +3689,7 @@
         <v>107.664385</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>191.40304599999999</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>684.05627800000002</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>98.179179000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>19.853853000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>179.29013499999999</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>620.14973899999995</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -3970,7 +3976,7 @@
         <v>31.241869999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -4011,7 +4017,7 @@
         <v>58.380809999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -4052,7 +4058,7 @@
         <v>73.538522</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -4093,7 +4099,7 @@
         <v>15.361072</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>252.41647499999999</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -4175,7 +4181,7 @@
         <v>64.190015000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -4216,7 +4222,7 @@
         <v>611.70663300000001</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -4257,7 +4263,7 @@
         <v>370.21644600000002</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -4298,7 +4304,7 @@
         <v>134.169522</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -4339,7 +4345,7 @@
         <v>170.16440399999999</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -4380,7 +4386,7 @@
         <v>170.84745100000001</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -4421,7 +4427,7 @@
         <v>37.640546999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -4462,7 +4468,7 @@
         <v>375.94035600000001</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -4503,7 +4509,7 @@
         <v>489.05092300000001</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -4544,7 +4550,7 @@
         <v>24.712071999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>92.572754000000003</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>12.155806999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -4667,7 +4673,7 @@
         <v>279.09021899999999</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -4708,7 +4714,7 @@
         <v>63.945394</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -4749,7 +4755,7 @@
         <v>118.39265</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -4790,7 +4796,7 @@
         <v>182.65201400000001</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>51.199404999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -4872,7 +4878,7 @@
         <v>314.65473600000001</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -4913,7 +4919,7 @@
         <v>166.71735899999999</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -4954,7 +4960,7 @@
         <v>8.7167320000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -4995,7 +5001,7 @@
         <v>152.72064599999999</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>109.605498</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -5077,7 +5083,7 @@
         <v>202.47062500000001</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -5118,7 +5124,7 @@
         <v>389.79455999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -5159,7 +5165,7 @@
         <v>568.56477700000005</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -5200,7 +5206,7 @@
         <v>223.69870599999999</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -5241,7 +5247,7 @@
         <v>139.87114700000001</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -5282,7 +5288,7 @@
         <v>81.645904000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -5323,7 +5329,7 @@
         <v>256.79791499999999</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -5364,7 +5370,7 @@
         <v>95.78313</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -5405,7 +5411,7 @@
         <v>156.90335099999999</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -5446,7 +5452,7 @@
         <v>396.337828</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>191.67502400000001</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -5528,7 +5534,7 @@
         <v>54.430923</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -5569,7 +5575,7 @@
         <v>42.214759999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -5610,7 +5616,7 @@
         <v>65.059972000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -5651,7 +5657,7 @@
         <v>59.059835999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -5692,7 +5698,7 @@
         <v>606.25028399999997</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -5733,7 +5739,7 @@
         <v>1217.045979</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -5774,7 +5780,7 @@
         <v>375.53034500000001</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -5815,7 +5821,7 @@
         <v>515.49155499999995</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -5856,7 +5862,7 @@
         <v>679.32207700000004</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -5897,7 +5903,7 @@
         <v>360.90303</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>279.63384200000002</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -5979,7 +5985,7 @@
         <v>87.708442000000005</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>141</v>
       </c>
@@ -6020,7 +6026,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>142</v>
       </c>
@@ -6061,7 +6067,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>143</v>
       </c>
@@ -6102,7 +6108,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>144</v>
       </c>
@@ -6143,7 +6149,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>145</v>
       </c>
@@ -6184,7 +6190,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>146</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -6266,7 +6272,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>148</v>
       </c>
@@ -6307,7 +6313,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -6348,7 +6354,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>150</v>
       </c>
@@ -6389,7 +6395,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -6430,7 +6436,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>152</v>
       </c>
@@ -6471,7 +6477,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>153</v>
       </c>
@@ -6512,7 +6518,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>154</v>
       </c>
@@ -6553,7 +6559,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>155</v>
       </c>
@@ -6594,7 +6600,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>156</v>
       </c>
@@ -6635,7 +6641,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>157</v>
       </c>
@@ -6676,7 +6682,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>158</v>
       </c>
@@ -6717,7 +6723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>159</v>
       </c>
@@ -6758,7 +6764,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>160</v>
       </c>
@@ -6799,7 +6805,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -6849,16 +6855,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC4EB9F-6BB2-4D9C-8BEB-97B376FF7802}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="4" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6875,10 +6884,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -6907,7 +6916,7 @@
         <v>42.371900826446279</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -6936,7 +6945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -6965,7 +6974,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -6994,231 +7003,303 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6">
+        <f>_xlfn.STDEV.P(home_range_data!J$2:J$122)</f>
+        <v>474.73692157594047</v>
+      </c>
+      <c r="C6">
+        <f>_xlfn.STDEV.P(home_range_data!K$2:K$122)</f>
+        <v>111.97343657982643</v>
+      </c>
+      <c r="D6">
+        <f>_xlfn.STDEV.P(home_range_data!L$2:L$122)</f>
+        <v>26.882760270601413</v>
+      </c>
+      <c r="E6">
+        <f>_xlfn.STDEV.P(home_range_data!M$2:M$122)</f>
+        <v>189.82601699105803</v>
+      </c>
+      <c r="F6">
+        <f>_xlfn.STDEV.P(home_range_data!G$2:G$122)</f>
+        <v>22.472735947748856</v>
+      </c>
+      <c r="G6">
+        <f>_xlfn.STDEV.P(home_range_data!H$2:H$122)</f>
+        <v>33.109917675116236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7">
+        <f>B6/SQRT(COUNT(home_range_data!J$2:J$122))</f>
+        <v>43.157901961449134</v>
+      </c>
+      <c r="C7">
+        <f>C6/SQRT(COUNT(home_range_data!K$2:K$122))</f>
+        <v>10.179403325438766</v>
+      </c>
+      <c r="D7">
+        <f>D6/SQRT(COUNT(home_range_data!L$2:L$122))</f>
+        <v>2.4438872973274011</v>
+      </c>
+      <c r="E7">
+        <f>E6/SQRT(COUNT(home_range_data!M$2:M$122))</f>
+        <v>17.256910635550728</v>
+      </c>
+      <c r="F7">
+        <f>F6/SQRT(COUNT(home_range_data!G$2:G$122))</f>
+        <v>2.042975995249896</v>
+      </c>
+      <c r="G7">
+        <f>G6/SQRT(COUNT(home_range_data!H$2:H$122))</f>
+        <v>3.0099925159196577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>138</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="str" cm="1">
-        <f t="array" ref="A10:A19">_xlfn._xlws.SORT(_xlfn.UNIQUE(home_range_data!E2:E143))</f>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="str" cm="1">
+        <f t="array" ref="A11:A20">_xlfn._xlws.SORT(_xlfn.UNIQUE(home_range_data!E2:E143))</f>
         <v>Site 1</v>
       </c>
-      <c r="B10" cm="1">
-        <f t="array" ref="B10:B19">COUNTIF(home_range_data!E2:E143,_xlfn.ANCHORARRAY(A10))</f>
+      <c r="B11" cm="1">
+        <f t="array" ref="B11:B20">COUNTIF(home_range_data!E2:E143,_xlfn.ANCHORARRAY(A11))</f>
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>176</v>
       </c>
-      <c r="E10">
-        <f>AVERAGE(_xlfn.ANCHORARRAY(B10))</f>
+      <c r="E11">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(B11))</f>
         <v>14.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="str">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
         <v>Site 10</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>175</v>
       </c>
-      <c r="E11">
-        <f>MIN(_xlfn.ANCHORARRAY(B10))</f>
+      <c r="E12">
+        <f>MIN(_xlfn.ANCHORARRAY(B11))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="str">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
         <v>Site 2</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>177</v>
       </c>
-      <c r="E12">
-        <f>MAX(_xlfn.ANCHORARRAY(B10))</f>
+      <c r="E13">
+        <f>MAX(_xlfn.ANCHORARRAY(B11))</f>
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="str">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
         <v>Site 3</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>178</v>
       </c>
-      <c r="E13">
-        <f>MEDIAN(_xlfn.ANCHORARRAY(B10))</f>
+      <c r="E14">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(B11))</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="str">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
         <v>Site 4</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="str">
+      <c r="D15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15">
+        <f>_xlfn.STDEV.P(_xlfn.ANCHORARRAY(B11))</f>
+        <v>10.952625256074453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
         <v>Site 5</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" t="str">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
         <v>Site 6</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" t="str">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
         <v>Site 7</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" t="str">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
         <v>Site 8</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" t="str">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
         <v>Site 9</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>129</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" t="str" cm="1">
-        <f t="array" ref="A23:A31">_xlfn._xlws.SORT(_xlfn.UNIQUE(home_range_data!C2:C143))</f>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="str" cm="1">
+        <f t="array" ref="A24:A32">_xlfn._xlws.SORT(_xlfn.UNIQUE(home_range_data!C2:C143))</f>
         <v>2020 Dry Season</v>
       </c>
-      <c r="B23" cm="1">
-        <f t="array" ref="B23:B31">COUNTIF(home_range_data!C2:C143,_xlfn.ANCHORARRAY(A23))</f>
+      <c r="B24" cm="1">
+        <f t="array" ref="B24:B32">COUNTIF(home_range_data!C2:C143,_xlfn.ANCHORARRAY(A24))</f>
         <v>7</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>176</v>
       </c>
-      <c r="E23">
-        <f>AVERAGE(_xlfn.ANCHORARRAY(B23))</f>
+      <c r="E24">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(B24))</f>
         <v>15.777777777777779</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" t="str">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
         <v>2021 Dry Season</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>175</v>
       </c>
-      <c r="E24">
-        <f>MIN(_xlfn.ANCHORARRAY(B23))</f>
+      <c r="E25">
+        <f>MIN(_xlfn.ANCHORARRAY(B24))</f>
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" t="str">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
         <v>2021 Early Wet Season</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>177</v>
       </c>
-      <c r="E25">
-        <f>MAX(_xlfn.ANCHORARRAY(B23))</f>
+      <c r="E26">
+        <f>MAX(_xlfn.ANCHORARRAY(B24))</f>
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" t="str">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
         <v>2021 Wet Season</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>178</v>
       </c>
-      <c r="E26">
-        <f>MEDIAN(_xlfn.ANCHORARRAY(B23))</f>
+      <c r="E27">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(B24))</f>
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" t="str">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
         <v>2022 Dry Season</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" t="str">
+      <c r="D28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E28">
+        <f>_xlfn.STDEV.P(_xlfn.ANCHORARRAY(B24))</f>
+        <v>5.593205754956986</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
         <v>2022 Early Wet Season</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" t="str">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
         <v>2022 Wet Season</v>
-      </c>
-      <c r="B29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" t="str">
-        <v>2023 Early Wet Season</v>
       </c>
       <c r="B30">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
+        <v>2023 Early Wet Season</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
         <v>2023 Wet Season</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>14</v>
       </c>
     </row>

</xml_diff>